<commit_message>
Unity 6.0 Addressable Scene 로딩 방식 변경으로 의한 SceneManager 구조수정
</commit_message>
<xml_diff>
--- a/DesignTable/Data/table명세서.xlsx
+++ b/DesignTable/Data/table명세서.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\ProjectT\DesignTable\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB8A5FDB-F052-4016-A98C-454488B7DE60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3315D591-23C0-4AE7-B39A-896DD8C2E95D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="716" uniqueCount="260">
   <si>
     <t>id</t>
     <phoneticPr fontId="6" type="noConversion"/>
@@ -1029,6 +1029,22 @@
   </si>
   <si>
     <t>{"UseListRule":true,"FindPKId" : ["skill_Id"],"PKIds":["skill_Id"]}</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>G_1024</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>SceneData</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>씬 데이터</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>SceneName</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
@@ -1710,10 +1726,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:K118"/>
+  <dimension ref="A1:K123"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView tabSelected="1" topLeftCell="A91" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J117" sqref="J117:K118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3375,7 +3391,7 @@
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A77" s="1">
-        <f t="shared" ref="A77:A118" si="1" xml:space="preserve"> ROW()</f>
+        <f t="shared" ref="A77:A123" si="1" xml:space="preserve"> ROW()</f>
         <v>77</v>
       </c>
     </row>
@@ -4248,10 +4264,100 @@
       </c>
       <c r="I118" s="11"/>
     </row>
+    <row r="119" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A119" s="1">
+        <f xml:space="preserve"> ROW()</f>
+        <v>119</v>
+      </c>
+    </row>
+    <row r="120" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A120" s="1">
+        <f t="shared" si="1"/>
+        <v>120</v>
+      </c>
+      <c r="B120" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="C120" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D120" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E120" s="6" t="s">
+        <v>258</v>
+      </c>
+      <c r="F120" s="6" t="s">
+        <v>257</v>
+      </c>
+      <c r="G120" s="6"/>
+      <c r="H120" s="6"/>
+      <c r="I120" s="6"/>
+      <c r="J120" s="6"/>
+      <c r="K120" s="6"/>
+    </row>
+    <row r="121" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A121" s="1">
+        <f t="shared" si="1"/>
+        <v>121</v>
+      </c>
+    </row>
+    <row r="122" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A122" s="1">
+        <f t="shared" si="1"/>
+        <v>122</v>
+      </c>
+      <c r="B122" s="9"/>
+      <c r="C122" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D122" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E122" s="10" t="s">
+        <v>259</v>
+      </c>
+      <c r="F122" s="10" t="s">
+        <v>259</v>
+      </c>
+      <c r="G122" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="H122" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I122" s="11"/>
+      <c r="K122" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="123" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A123" s="1">
+        <f t="shared" si="1"/>
+        <v>123</v>
+      </c>
+      <c r="B123" s="9"/>
+      <c r="C123" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D123" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E123" s="10" t="s">
+        <v>254</v>
+      </c>
+      <c r="F123" s="10" t="s">
+        <v>254</v>
+      </c>
+      <c r="G123" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="I123" s="11"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G52:G53 G57:G67 G40:G48 G71:G76 G80:G85 G89:G91 G95:G100 G104:G108 G15:G36 G112:G114 G5:G11 G117:G118" xr:uid="{264C1E52-5B28-48FA-83C0-DDC263029AB9}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G52:G53 G57:G67 G40:G48 G71:G76 G80:G85 G89:G91 G95:G100 G104:G108 G15:G36 G112:G114 G5:G11 G117:G118 G122:G123" xr:uid="{264C1E52-5B28-48FA-83C0-DDC263029AB9}">
       <formula1>DataType</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>